<commit_message>
mahasiswa asing, dosen industri, pagelaran dtps, produk/jasa
</commit_message>
<xml_diff>
--- a/formatted/sapto_seleksi_mhs_baru (F).xlsx
+++ b/formatted/sapto_seleksi_mhs_baru (F).xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet 2" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Worksheet'!$B$1:$L$17</definedName>
@@ -1384,7 +1385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" hidden="true">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -1428,6 +1429,15 @@
     <filterColumn colId="0">
       <filters>
         <filter val="S-1 T.MESIN"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="3">
+      <filters>
+        <filter val="TS-4"/>
+        <filter val="TS-3"/>
+        <filter val="TS-2"/>
+        <filter val="TS-1"/>
+        <filter val="TS"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -1443,4 +1453,115 @@
     <firstFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1">
+        <v>801</v>
+      </c>
+      <c r="D1">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2">
+        <v>666</v>
+      </c>
+      <c r="G2">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <v>232</v>
+      </c>
+      <c r="C3">
+        <v>4328</v>
+      </c>
+      <c r="D3">
+        <v>232</v>
+      </c>
+      <c r="E3">
+        <v>192</v>
+      </c>
+      <c r="G3">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4">
+        <v>227</v>
+      </c>
+      <c r="C4">
+        <v>4060</v>
+      </c>
+      <c r="D4">
+        <v>227</v>
+      </c>
+      <c r="E4">
+        <v>203</v>
+      </c>
+      <c r="G4">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>297</v>
+      </c>
+      <c r="C5">
+        <v>4937</v>
+      </c>
+      <c r="D5">
+        <v>297</v>
+      </c>
+      <c r="E5">
+        <v>270</v>
+      </c>
+      <c r="G5">
+        <v>959</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>